<commit_message>
Complete draft of ilemt_calibration.docx, with abstract, introduction and conclusion. Checked cross references for figures, equations and tables. Fixed page breaks again.
</commit_message>
<xml_diff>
--- a/calibration/residue_stats.xlsx
+++ b/calibration/residue_stats.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robma\Documents\Work\ilemt_papers\calibration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF49F08C-CC11-43FE-AEB7-434C71362921}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD22F275-4E62-4879-98C4-2DDE992D19D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6996" yWindow="3192" windowWidth="34560" windowHeight="19140" xr2:uid="{70342531-14B4-4B61-B0C0-6FE86FF8B2FA}"/>
+    <workbookView xWindow="6144" yWindow="6144" windowWidth="34560" windowHeight="19140" xr2:uid="{70342531-14B4-4B61-B0C0-6FE86FF8B2FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
   <si>
     <t>Calibration type</t>
   </si>
@@ -59,6 +59,9 @@
   </si>
   <si>
     <t>Dipole approx</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -749,7 +752,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection sqref="A1:D6"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -789,7 +792,9 @@
       <c r="A3" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="8"/>
+      <c r="B3" s="8" t="s">
+        <v>7</v>
+      </c>
       <c r="C3" s="22">
         <f>'[1]Cal stats'!$B$6</f>
         <v>5.4206423616771568E-3</v>
@@ -819,7 +824,9 @@
       <c r="A5" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="8"/>
+      <c r="B5" s="8" t="s">
+        <v>7</v>
+      </c>
       <c r="C5" s="11">
         <f>'[1]Cal stats'!$B$4</f>
         <v>0.20807749014095389</v>

</xml_diff>

<commit_message>
Various small formatting tweaks from proofreading.
</commit_message>
<xml_diff>
--- a/calibration/residue_stats.xlsx
+++ b/calibration/residue_stats.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robma\Documents\Work\ilemt_papers\calibration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD22F275-4E62-4879-98C4-2DDE992D19D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CB0ED0A-7E40-457D-AD7B-CEAA24B2E48E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6144" yWindow="6144" windowWidth="34560" windowHeight="19140" xr2:uid="{70342531-14B4-4B61-B0C0-6FE86FF8B2FA}"/>
+    <workbookView xWindow="380" yWindow="380" windowWidth="28800" windowHeight="15460" xr2:uid="{70342531-14B4-4B61-B0C0-6FE86FF8B2FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -268,7 +268,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
@@ -287,10 +287,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -299,10 +296,9 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
@@ -312,11 +308,11 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -334,10 +330,10 @@
     <xf numFmtId="10" fontId="2" fillId="2" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -346,10 +342,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -371,7 +367,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Error stats"/>
@@ -415,7 +411,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Error stats"/>
@@ -423,7 +419,13 @@
       <sheetName val="Cal stats"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
+      <sheetData sheetId="0">
+        <row r="4">
+          <cell r="B4">
+            <v>0.26305582094218294</v>
+          </cell>
+        </row>
+      </sheetData>
       <sheetData sheetId="1"/>
       <sheetData sheetId="2">
         <row r="4">
@@ -453,9 +455,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -493,7 +495,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -599,7 +601,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -741,7 +743,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -752,128 +754,128 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.77734375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="11.44140625" style="9" customWidth="1"/>
+    <col min="1" max="1" width="11.81640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="11.453125" style="3" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
-    <col min="4" max="4" width="8.77734375" customWidth="1"/>
-    <col min="5" max="5" width="7.77734375" customWidth="1"/>
+    <col min="4" max="4" width="8.81640625" customWidth="1"/>
+    <col min="5" max="5" width="7.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="14"/>
-      <c r="B1" s="20"/>
-      <c r="C1" s="29" t="s">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="12" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="12"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="30"/>
+      <c r="D1" s="28"/>
       <c r="E1" s="5"/>
     </row>
-    <row r="2" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="19" t="s">
+    <row r="2" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="12"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="31" t="s">
+      <c r="E2" s="11"/>
+    </row>
+    <row r="3" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="29" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="22">
+      <c r="C3" s="20">
         <f>'[1]Cal stats'!$B$6</f>
         <v>5.4206423616771568E-3</v>
       </c>
-      <c r="D3" s="22">
+      <c r="D3" s="20">
         <f>'[2]Cal stats'!$B$6</f>
         <v>5.154698098915049E-3</v>
       </c>
-      <c r="E3" s="15"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="32"/>
+      <c r="E3" s="13"/>
+    </row>
+    <row r="4" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="30"/>
       <c r="B4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="26">
+      <c r="C4" s="24">
         <f>'[1]Cal stats'!$B$7</f>
         <v>7.6404098323088398E-3</v>
       </c>
-      <c r="D4" s="25">
+      <c r="D4" s="23">
         <f>'[2]Cal stats'!$B$7</f>
         <v>1.1563648163885921E-2</v>
       </c>
-      <c r="E4" s="15"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="27" t="s">
+      <c r="E4" s="13"/>
+    </row>
+    <row r="5" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="25" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="10">
         <f>'[1]Cal stats'!$B$4</f>
         <v>0.20807749014095389</v>
       </c>
-      <c r="D5" s="23">
+      <c r="D5" s="21">
         <f>'[2]Cal stats'!$B$4</f>
         <v>7.092240261140333E-3</v>
       </c>
-      <c r="E5" s="15"/>
-    </row>
-    <row r="6" spans="1:9" s="2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="28"/>
+      <c r="E5" s="13"/>
+    </row>
+    <row r="6" spans="1:9" s="2" customFormat="1" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="26"/>
       <c r="B6" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="9">
         <f>'[1]Cal stats'!$B$5</f>
         <v>0.36646059248309831</v>
       </c>
-      <c r="D6" s="24">
+      <c r="D6" s="22">
         <f>'[2]Cal stats'!$B$5</f>
         <v>1.8890501981792325E-2</v>
       </c>
-      <c r="E6" s="16"/>
-    </row>
-    <row r="7" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E6" s="14"/>
+    </row>
+    <row r="7" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>

</xml_diff>